<commit_message>
Udate inception sheet for inception phase
</commit_message>
<xml_diff>
--- a/Teleologies/Inception/InceptionSheet.xlsx
+++ b/Teleologies/Inception/InceptionSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frigo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frigo\Desktop\wsl\kdi\Trentino-territory\Teleologies\Inception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5D99C9-F616-48D6-A757-0342EFC0E2EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E861FF6-0A79-4481-ADF0-A38973C1510D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>Persona</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>company</t>
+  </si>
+  <si>
+    <t>Which attractions are owned by a company?</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>company, attraction</t>
   </si>
 </sst>
 </file>
@@ -214,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -237,11 +246,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -262,14 +293,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,8 +531,8 @@
   </sheetPr>
   <dimension ref="A1:W999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -606,7 +647,7 @@
       <c r="D5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="13" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="7"/>
@@ -735,22 +776,30 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="A14" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
     </row>
     <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
     </row>
     <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E16" s="9"/>
@@ -768,29 +817,29 @@
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>

</xml_diff>